<commit_message>
CSS edits + searchbar
</commit_message>
<xml_diff>
--- a/persone_famose.xlsx
+++ b/persone_famose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maric\Desktop\events_manager_00\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzomarinaro/Desktop/eventsmanager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE2C20D-F0A8-469D-BD15-A541594B8A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1662985B-D2AD-9C47-A88C-508FA9E7D271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{FC40FD77-30A6-43AB-9451-9238216CD433}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="23020" windowHeight="12220" xr2:uid="{FC40FD77-30A6-43AB-9451-9238216CD433}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="17">
   <si>
     <t>nome</t>
   </si>
@@ -135,7 +135,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -447,15 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA81E561-6118-4CAF-AAF7-9A777CFE5E1F}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -478,7 +478,7 @@
         <v>francesco_totti</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -490,7 +490,7 @@
         <v>donald_trump</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -502,7 +502,7 @@
         <v>manuela_arcuri</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -514,7 +514,7 @@
         <v>elsa_frozen</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -526,7 +526,7 @@
         <v>giorgia_meloni</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -538,7 +538,7 @@
         <v>napoleone_bonaparte</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -547,6 +547,258 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
+        <v>gruppo_pooh</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="str">
+        <f>_xlfn.CONCAT(A9,"_",B9)</f>
+        <v>francesco_totti</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" ref="C10:C15" si="1">_xlfn.CONCAT(A10,"_",B10)</f>
+        <v>donald_trump</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>manuela_arcuri</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>elsa_frozen</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>giorgia_meloni</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>napoleone_bonaparte</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>gruppo_pooh</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xlfn.CONCAT(A16,"_",B16)</f>
+        <v>francesco_totti</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" ref="C17:C22" si="2">_xlfn.CONCAT(A17,"_",B17)</f>
+        <v>donald_trump</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="2"/>
+        <v>manuela_arcuri</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="2"/>
+        <v>elsa_frozen</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="2"/>
+        <v>giorgia_meloni</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="2"/>
+        <v>napoleone_bonaparte</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="2"/>
+        <v>gruppo_pooh</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT(A23,"_",B23)</f>
+        <v>francesco_totti</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" ref="C24:C29" si="3">_xlfn.CONCAT(A24,"_",B24)</f>
+        <v>donald_trump</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="3"/>
+        <v>manuela_arcuri</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="3"/>
+        <v>elsa_frozen</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="3"/>
+        <v>giorgia_meloni</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="3"/>
+        <v>napoleone_bonaparte</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="3"/>
         <v>gruppo_pooh</v>
       </c>
     </row>

</xml_diff>